<commit_message>
Fix #4004 Model EMX_MODEL.xlsx import error
</commit_message>
<xml_diff>
--- a/molgenis-model-registry/src/test/resources/EMX_MODEL.xlsx
+++ b/molgenis-model-registry/src/test/resources/EMX_MODEL.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15540" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="73">
   <si>
     <t>name</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>molgenis_home,molgenis_github,molgenis_demo</t>
+  </si>
+  <si>
+    <t>unique_</t>
   </si>
 </sst>
 </file>
@@ -824,17 +827,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="57" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -848,7 +851,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -878,15 +881,15 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -900,7 +903,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -914,7 +917,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -928,7 +931,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -942,7 +945,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>46</v>
       </c>
@@ -969,424 +972,430 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>46</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="F2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>46</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>57</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
       <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
         <v>0</v>
       </c>
-      <c r="J4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>57</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="J5" t="b">
-        <v>1</v>
-      </c>
       <c r="K5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="L5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>57</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="F6" t="b">
+      <c r="G6" t="b">
         <v>0</v>
       </c>
-      <c r="J6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>58</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
       <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" t="b">
         <v>0</v>
       </c>
-      <c r="J7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>58</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="J8" t="b">
-        <v>1</v>
-      </c>
       <c r="K8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="L8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>58</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F9" t="b">
+      <c r="G9" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>50</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>58</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>7</v>
       </c>
-      <c r="F10" t="b">
+      <c r="G10" t="b">
         <v>0</v>
       </c>
-      <c r="J10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="K10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>59</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>7</v>
       </c>
-      <c r="E11" t="b">
-        <v>1</v>
-      </c>
       <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" t="b">
         <v>0</v>
       </c>
-      <c r="J11" t="b">
-        <v>1</v>
-      </c>
       <c r="K11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="L11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>58</v>
       </c>
-      <c r="F12" t="b">
+      <c r="G12" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>59</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>8</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>46</v>
       </c>
-      <c r="F13" t="b">
+      <c r="G13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>59</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>59</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>59</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>59</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>59</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>59</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>59</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>59</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>59</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>59</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>47</v>
       </c>
-      <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>17</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>59</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" t="s">
         <v>18</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>59</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="1"/>
       <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1407,13 +1416,13 @@
       <selection activeCell="B2" sqref="B2:B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1421,7 +1430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1429,7 +1438,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1437,7 +1446,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1445,7 +1454,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1453,7 +1462,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1461,7 +1470,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1469,7 +1478,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1477,7 +1486,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1485,7 +1494,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1493,7 +1502,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1501,7 +1510,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -1509,7 +1518,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1517,7 +1526,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1525,7 +1534,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -1533,7 +1542,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -1541,7 +1550,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1549,7 +1558,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -1557,7 +1566,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -1565,7 +1574,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -1592,16 +1601,16 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="40.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>48</v>
       </c>
@@ -1621,7 +1630,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>68</v>
       </c>
@@ -1641,7 +1650,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>69</v>
       </c>
@@ -1661,7 +1670,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
Fix missing idAttribute import error by using fully qualified entity names
</commit_message>
<xml_diff>
--- a/molgenis-model-registry/src/test/resources/EMX_MODEL.xlsx
+++ b/molgenis-model-registry/src/test/resources/EMX_MODEL.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15540" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15540" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="5" r:id="rId1"/>
     <sheet name="entities" sheetId="3" r:id="rId2"/>
     <sheet name="attributes" sheetId="4" r:id="rId3"/>
-    <sheet name="molgenisfieldtypes" sheetId="1" r:id="rId4"/>
+    <sheet name="emx_molgenisfieldtypes" sheetId="1" r:id="rId4"/>
     <sheet name="tags" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="77">
   <si>
     <t>name</t>
   </si>
@@ -242,6 +242,18 @@
   </si>
   <si>
     <t>unique_</t>
+  </si>
+  <si>
+    <t>emx_molgenisfieldtypes</t>
+  </si>
+  <si>
+    <t>emx_packagesEMX</t>
+  </si>
+  <si>
+    <t>emx_entitiesEMX</t>
+  </si>
+  <si>
+    <t>emx_attributesEMX</t>
   </si>
 </sst>
 </file>
@@ -974,16 +986,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -1045,7 +1057,7 @@
         <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -1062,7 +1074,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -1075,7 +1087,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -1095,7 +1107,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -1112,7 +1124,7 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -1129,7 +1141,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -1149,7 +1161,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -1166,13 +1178,13 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
         <v>61</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
@@ -1183,7 +1195,7 @@
         <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -1200,7 +1212,7 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -1223,13 +1235,13 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="G12" t="b">
         <v>0</v>
@@ -1240,13 +1252,13 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="G13" t="b">
         <v>0</v>
@@ -1257,7 +1269,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
@@ -1270,7 +1282,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D15" t="s">
         <v>47</v>
@@ -1281,7 +1293,7 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D16" t="s">
         <v>47</v>
@@ -1292,7 +1304,7 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D17" t="s">
         <v>47</v>
@@ -1303,7 +1315,7 @@
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D18" t="s">
         <v>47</v>
@@ -1314,7 +1326,7 @@
         <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D19" t="s">
         <v>47</v>
@@ -1325,7 +1337,7 @@
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D20" t="s">
         <v>47</v>
@@ -1336,7 +1348,7 @@
         <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D21" t="s">
         <v>47</v>
@@ -1349,7 +1361,7 @@
         <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D22" t="s">
         <v>47</v>
@@ -1360,7 +1372,7 @@
         <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D23" t="s">
         <v>47</v>
@@ -1373,7 +1385,7 @@
         <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D24" t="s">
         <v>47</v>
@@ -1389,7 +1401,7 @@
         <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
@@ -1412,8 +1424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>